<commit_message>
Validaciones de facturacion, consulta de BL, cambios en el servicio para el control de historial de ISOType
</commit_message>
<xml_diff>
--- a/CEPA.CCO.UI.Web/Anexo_export.xlsx
+++ b/CEPA.CCO.UI.Web/Anexo_export.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$M$5</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$O$5</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>BUQUE:</t>
   </si>
@@ -119,6 +119,15 @@
   </si>
   <si>
     <t>AGENCIA:</t>
+  </si>
+  <si>
+    <t>VACIADO</t>
+  </si>
+  <si>
+    <t>F. VACIADO</t>
+  </si>
+  <si>
+    <t>F. VACIADO Y LLENADO</t>
   </si>
 </sst>
 </file>
@@ -208,7 +217,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -358,6 +367,69 @@
         <color indexed="64"/>
       </left>
       <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -373,7 +445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -384,6 +456,21 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="8" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="8" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -417,59 +504,68 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="8" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="8" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="4" fontId="8" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="8" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="8" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="8" fillId="3" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="8" fillId="3" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -801,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,211 +908,243 @@
     <col min="1" max="1" width="6.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="1" customWidth="1"/>
     <col min="8" max="11" width="11.42578125" style="1"/>
-    <col min="12" max="12" width="16.140625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="8" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" style="8" customWidth="1"/>
+    <col min="14" max="15" width="16.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
     </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
     </row>
-    <row r="3" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
+    <row r="3" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
     </row>
-    <row r="4" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
+    <row r="4" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
     </row>
-    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
+    <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="8"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="13"/>
     </row>
-    <row r="7" spans="1:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="11"/>
+    <row r="7" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="16"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="12" t="s">
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="12" t="s">
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="15" t="s">
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="M8" s="16"/>
+      <c r="O8" s="37"/>
     </row>
-    <row r="9" spans="1:13" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+    <row r="9" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="23" t="s">
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" s="35"/>
+      <c r="N9" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="M9" s="24" t="s">
+      <c r="O9" s="32" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
+    <row r="10" spans="1:15" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="21"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="29"/>
-      <c r="H10" s="30" t="s">
+      <c r="H10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="30" t="s">
+      <c r="I10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J10" s="30" t="s">
+      <c r="J10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="30" t="s">
+      <c r="K10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L10" s="31"/>
-      <c r="M10" s="32"/>
+      <c r="L10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="31"/>
+      <c r="O10" s="33"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A1:M5"/>
-    <mergeCell ref="A6:M7"/>
+  <mergeCells count="17">
+    <mergeCell ref="I8:M8"/>
+    <mergeCell ref="A1:O5"/>
+    <mergeCell ref="A6:O7"/>
     <mergeCell ref="A8:D8"/>
-    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N8:O8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
@@ -1024,11 +1152,11 @@
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="H9:K9"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
     <mergeCell ref="E8:H8"/>
-    <mergeCell ref="I8:K8"/>
     <mergeCell ref="F9:F10"/>
+    <mergeCell ref="L9:M9"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.57999999999999996" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="56" orientation="portrait" r:id="rId1"/>

</xml_diff>